<commit_message>
Se corrijio bug de impresion de informacion de TIPOS DE PROCESO
</commit_message>
<xml_diff>
--- a/dist/datos/codigos_cumple.xlsx
+++ b/dist/datos/codigos_cumple.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7691"/>
+  <dimension ref="A1:C7690"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -93433,19 +93433,6 @@
         </is>
       </c>
     </row>
-    <row r="7691">
-      <c r="A7691" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7691" t="inlineStr">
-        <is>
-          <t>cumple</t>
-        </is>
-      </c>
-      <c r="C7691" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregaron filtros para NOM004 y NOM020
</commit_message>
<xml_diff>
--- a/dist/datos/codigos_cumple.xlsx
+++ b/dist/datos/codigos_cumple.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7690"/>
+  <dimension ref="A1:C7716"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,14 +512,10 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SIN</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -784,11 +780,7 @@
       <c r="A28" t="n">
         <v>534503</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -1001,11 +993,7 @@
       <c r="A47" t="n">
         <v>699402</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -2274,7 +2262,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -2304,7 +2292,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2319,14 +2307,10 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -2337,11 +2321,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -2695,11 +2675,7 @@
       <c r="A185" t="n">
         <v>2111280</v>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B185" t="inlineStr"/>
       <c r="C185" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -2783,7 +2759,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -2864,11 +2840,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -2876,14 +2848,10 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -3119,11 +3087,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -3131,14 +3095,10 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -3146,14 +3106,10 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -3161,14 +3117,10 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -3176,14 +3128,10 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -3191,14 +3139,10 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C223" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -3206,14 +3150,10 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C224" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -3236,14 +3176,10 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C226" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -3251,14 +3187,10 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C227" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -3266,14 +3198,10 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C228" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -3824,14 +3752,10 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C274" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -3839,14 +3763,10 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C275" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -3854,14 +3774,10 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C276" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -3869,14 +3785,10 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C277" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -3884,14 +3796,10 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C278" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -3899,14 +3807,10 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>inSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C279" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -3914,14 +3818,10 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>insTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C280" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -3929,14 +3829,10 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C281" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -3944,14 +3840,10 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C282" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -3959,14 +3851,10 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C283" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -3974,14 +3862,10 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C284" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -3989,14 +3873,10 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C285" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -4004,14 +3884,10 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C286" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -4019,14 +3895,10 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C287" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -4034,14 +3906,10 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C288" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -4194,7 +4062,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -4381,7 +4249,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -4407,7 +4275,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -4420,11 +4288,7 @@
       <c r="A316" t="n">
         <v>2354662</v>
       </c>
-      <c r="B316" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B316" t="inlineStr"/>
       <c r="C316" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -5053,14 +4917,10 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C365" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="n">
@@ -5068,14 +4928,10 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C366" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="n">
@@ -5083,14 +4939,10 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C367" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" t="n">
@@ -5154,7 +5006,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>No exprimir, no centrifugar y secado en línea a la sombra.</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
@@ -5515,11 +5367,7 @@
       <c r="A401" t="n">
         <v>2454976</v>
       </c>
-      <c r="B401" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B401" t="inlineStr"/>
       <c r="C401" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -6847,7 +6695,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
@@ -7000,7 +6848,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>REVISADO</t>
+          <t>IMPORTADOR</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
@@ -7922,14 +7770,10 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C588" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr"/>
     </row>
     <row r="589">
       <c r="A589" t="n">
@@ -8056,7 +7900,7 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
+          <t>CUMPLE</t>
         </is>
       </c>
       <c r="C598" t="inlineStr"/>
@@ -8197,14 +8041,10 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C609" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr"/>
     </row>
     <row r="610">
       <c r="A610" t="n">
@@ -8640,14 +8480,10 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C646" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr"/>
     </row>
     <row r="647">
       <c r="A647" t="n">
@@ -8655,14 +8491,10 @@
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C647" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr"/>
     </row>
     <row r="648">
       <c r="A648" t="n">
@@ -8670,14 +8502,10 @@
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C648" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr"/>
     </row>
     <row r="649">
       <c r="A649" t="n">
@@ -8685,14 +8513,10 @@
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES, INSUMOS, IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C649" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr"/>
     </row>
     <row r="650">
       <c r="A650" t="n">
@@ -9093,14 +8917,10 @@
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C681" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr"/>
     </row>
     <row r="682">
       <c r="A682" t="n">
@@ -9215,14 +9035,10 @@
       </c>
       <c r="B691" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C691" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr"/>
     </row>
     <row r="692">
       <c r="A692" t="n">
@@ -9230,14 +9046,10 @@
       </c>
       <c r="B692" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C692" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr"/>
     </row>
     <row r="693">
       <c r="A693" t="n">
@@ -9245,14 +9057,10 @@
       </c>
       <c r="B693" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C693" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr"/>
     </row>
     <row r="694">
       <c r="A694" t="n">
@@ -9260,14 +9068,10 @@
       </c>
       <c r="B694" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C694" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr"/>
     </row>
     <row r="695">
       <c r="A695" t="n">
@@ -10189,11 +9993,7 @@
       <c r="A767" t="n">
         <v>2665773</v>
       </c>
-      <c r="B767" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B767" t="inlineStr"/>
       <c r="C767" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -10829,7 +10629,7 @@
       </c>
       <c r="B821" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C821" t="inlineStr">
@@ -10870,14 +10670,10 @@
       </c>
       <c r="B824" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C824" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr"/>
     </row>
     <row r="825">
       <c r="A825" t="n">
@@ -10982,7 +10778,7 @@
       </c>
       <c r="B832" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
         </is>
       </c>
       <c r="C832" t="inlineStr">
@@ -11075,14 +10871,10 @@
       </c>
       <c r="B839" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C839" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr"/>
     </row>
     <row r="840">
       <c r="A840" t="n">
@@ -11502,7 +11294,7 @@
       </c>
       <c r="B872" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>INSTRUCCIONES</t>
         </is>
       </c>
       <c r="C872" t="inlineStr">
@@ -11515,11 +11307,7 @@
       <c r="A873" t="n">
         <v>2708563</v>
       </c>
-      <c r="B873" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B873" t="inlineStr"/>
       <c r="C873" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -11530,11 +11318,7 @@
       <c r="A874" t="n">
         <v>2708564</v>
       </c>
-      <c r="B874" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B874" t="inlineStr"/>
       <c r="C874" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -11908,14 +11692,10 @@
       </c>
       <c r="B906" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECAR COLGADO A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C906" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr"/>
     </row>
     <row r="907">
       <c r="A907" t="n">
@@ -11978,10 +11758,14 @@
       </c>
       <c r="B912" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
-        </is>
-      </c>
-      <c r="C912" t="inlineStr"/>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
     </row>
     <row r="913">
       <c r="A913" t="n">
@@ -13576,7 +13360,7 @@
       </c>
       <c r="B1042" t="inlineStr">
         <is>
-          <t>IMPORTADOR ,PAIS</t>
+          <t>SIN</t>
         </is>
       </c>
       <c r="C1042" t="inlineStr">
@@ -13773,14 +13557,10 @@
       </c>
       <c r="B1057" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C1057" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr"/>
     </row>
     <row r="1058">
       <c r="A1058" t="n">
@@ -14704,14 +14484,10 @@
       </c>
       <c r="B1134" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C1134" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr"/>
     </row>
     <row r="1135">
       <c r="A1135" t="n">
@@ -14719,14 +14495,10 @@
       </c>
       <c r="B1135" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C1135" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr"/>
     </row>
     <row r="1136">
       <c r="A1136" t="n">
@@ -14737,11 +14509,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C1136" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C1136" t="inlineStr"/>
     </row>
     <row r="1137">
       <c r="A1137" t="n">
@@ -14749,14 +14517,10 @@
       </c>
       <c r="B1137" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C1137" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr"/>
     </row>
     <row r="1138">
       <c r="A1138" t="n">
@@ -15367,11 +15131,7 @@
       <c r="A1189" t="n">
         <v>2908940</v>
       </c>
-      <c r="B1189" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B1189" t="inlineStr"/>
       <c r="C1189" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -15488,14 +15248,10 @@
       </c>
       <c r="B1198" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C1198" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr"/>
     </row>
     <row r="1199">
       <c r="A1199" t="n">
@@ -15962,7 +15718,7 @@
       </c>
       <c r="B1236" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
+          <t>PAIS,IMPORTADOR</t>
         </is>
       </c>
       <c r="C1236" t="inlineStr">
@@ -15977,14 +15733,10 @@
       </c>
       <c r="B1237" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C1237" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr"/>
     </row>
     <row r="1238">
       <c r="A1238" t="n">
@@ -16974,11 +16726,7 @@
       <c r="A1318" t="n">
         <v>2955012</v>
       </c>
-      <c r="B1318" t="inlineStr">
-        <is>
-          <t>INSUMOS</t>
-        </is>
-      </c>
+      <c r="B1318" t="inlineStr"/>
       <c r="C1318" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -17384,11 +17132,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C1353" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C1353" t="inlineStr"/>
     </row>
     <row r="1354">
       <c r="A1354" t="n">
@@ -19214,7 +18958,7 @@
       </c>
       <c r="B1504" t="inlineStr">
         <is>
-          <t>REVISADO</t>
+          <t>IMPORTADOR</t>
         </is>
       </c>
       <c r="C1504" t="inlineStr">
@@ -19268,11 +19012,7 @@
       <c r="A1508" t="n">
         <v>4004970</v>
       </c>
-      <c r="B1508" t="inlineStr">
-        <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
+      <c r="B1508" t="inlineStr"/>
       <c r="C1508" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -19724,14 +19464,10 @@
       </c>
       <c r="B1546" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C1546" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1546" t="inlineStr"/>
     </row>
     <row r="1547">
       <c r="A1547" t="n">
@@ -19951,11 +19687,7 @@
       <c r="A1565" t="n">
         <v>4016598</v>
       </c>
-      <c r="B1565" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
+      <c r="B1565" t="inlineStr"/>
       <c r="C1565" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -20494,7 +20226,7 @@
       </c>
       <c r="B1608" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C1608" t="inlineStr">
@@ -21755,11 +21487,7 @@
       <c r="A1709" t="n">
         <v>4067032</v>
       </c>
-      <c r="B1709" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B1709" t="inlineStr"/>
       <c r="C1709" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -22995,7 +22723,7 @@
       </c>
       <c r="B1807" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C1807" t="inlineStr">
@@ -23378,7 +23106,7 @@
       </c>
       <c r="B1840" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
+          <t>SIN</t>
         </is>
       </c>
       <c r="C1840" t="inlineStr">
@@ -23393,14 +23121,10 @@
       </c>
       <c r="B1841" t="inlineStr">
         <is>
-          <t>IMPORTADOR EDAD RECOMENDADA</t>
-        </is>
-      </c>
-      <c r="C1841" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1841" t="inlineStr"/>
     </row>
     <row r="1842">
       <c r="A1842" t="n">
@@ -23534,14 +23258,10 @@
       </c>
       <c r="B1852" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C1852" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1852" t="inlineStr"/>
     </row>
     <row r="1853">
       <c r="A1853" t="n">
@@ -23652,7 +23372,7 @@
       </c>
       <c r="B1862" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C1862" t="inlineStr">
@@ -24586,14 +24306,10 @@
       </c>
       <c r="B1940" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C1940" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C1940" t="inlineStr"/>
     </row>
     <row r="1941">
       <c r="A1941" t="n">
@@ -24671,14 +24387,10 @@
       </c>
       <c r="B1947" t="inlineStr">
         <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
-      <c r="C1947" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C1947" t="inlineStr"/>
     </row>
     <row r="1948">
       <c r="A1948" t="n">
@@ -25099,7 +24811,7 @@
       </c>
       <c r="B1983" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
+          <t>IMPORTADOR</t>
         </is>
       </c>
       <c r="C1983" t="inlineStr">
@@ -25125,7 +24837,7 @@
       </c>
       <c r="B1985" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C1985" t="inlineStr">
@@ -25143,11 +24855,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C1986" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C1986" t="inlineStr"/>
     </row>
     <row r="1987">
       <c r="A1987" t="n">
@@ -25417,14 +25125,10 @@
       </c>
       <c r="B2009" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C2009" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C2009" t="inlineStr"/>
     </row>
     <row r="2010">
       <c r="A2010" t="n">
@@ -25435,11 +25139,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C2010" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C2010" t="inlineStr"/>
     </row>
     <row r="2011">
       <c r="A2011" t="n">
@@ -25572,11 +25272,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C2021" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C2021" t="inlineStr"/>
     </row>
     <row r="2022">
       <c r="A2022" t="n">
@@ -26051,7 +25747,7 @@
       </c>
       <c r="B2059" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>SIN ETIQUETA</t>
         </is>
       </c>
       <c r="C2059" t="inlineStr">
@@ -26769,7 +26465,7 @@
       </c>
       <c r="B2117" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2117" t="inlineStr">
@@ -28466,7 +28162,7 @@
       </c>
       <c r="B2256" t="inlineStr">
         <is>
-          <t>INSUMOS, IMPORTADOR</t>
+          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
         </is>
       </c>
       <c r="C2256" t="inlineStr">
@@ -28870,14 +28566,10 @@
       </c>
       <c r="B2288" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C2288" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C2288" t="inlineStr"/>
     </row>
     <row r="2289">
       <c r="A2289" t="n">
@@ -29664,11 +29356,7 @@
       <c r="A2348" t="n">
         <v>4313875</v>
       </c>
-      <c r="B2348" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B2348" t="inlineStr"/>
       <c r="C2348" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -30051,11 +29739,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C2378" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C2378" t="inlineStr"/>
     </row>
     <row r="2379">
       <c r="A2379" t="n">
@@ -30494,11 +30178,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C2415" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C2415" t="inlineStr"/>
     </row>
     <row r="2416">
       <c r="A2416" t="n">
@@ -30920,7 +30600,7 @@
       </c>
       <c r="B2450" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2450" t="inlineStr">
@@ -31007,11 +30687,7 @@
       <c r="A2457" t="n">
         <v>4336854</v>
       </c>
-      <c r="B2457" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B2457" t="inlineStr"/>
       <c r="C2457" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -31039,7 +30715,7 @@
       </c>
       <c r="B2459" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>INSTRUCCIONES</t>
         </is>
       </c>
       <c r="C2459" t="inlineStr">
@@ -31209,11 +30885,7 @@
       <c r="A2471" t="n">
         <v>4340941</v>
       </c>
-      <c r="B2471" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B2471" t="inlineStr"/>
       <c r="C2471" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -31739,7 +31411,7 @@
       </c>
       <c r="B2515" t="inlineStr">
         <is>
-          <t>No exprimir, no centrifugar y secado en línea a la sombra.</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2515" t="inlineStr">
@@ -31752,11 +31424,7 @@
       <c r="A2516" t="n">
         <v>4349762</v>
       </c>
-      <c r="B2516" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B2516" t="inlineStr"/>
       <c r="C2516" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -32239,7 +31907,7 @@
       </c>
       <c r="B2555" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2555" t="inlineStr">
@@ -33176,7 +32844,7 @@
       </c>
       <c r="B2634" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2634" t="inlineStr">
@@ -33191,7 +32859,7 @@
       </c>
       <c r="B2635" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2635" t="inlineStr">
@@ -33206,7 +32874,7 @@
       </c>
       <c r="B2636" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2636" t="inlineStr">
@@ -33236,7 +32904,7 @@
       </c>
       <c r="B2638" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2638" t="inlineStr">
@@ -34149,7 +33817,7 @@
       </c>
       <c r="B2713" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2713" t="inlineStr">
@@ -35898,7 +35566,7 @@
       </c>
       <c r="B2852" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2852" t="inlineStr">
@@ -36049,11 +35717,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C2864" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C2864" t="inlineStr"/>
     </row>
     <row r="2865">
       <c r="A2865" t="n">
@@ -36444,14 +36108,10 @@
       </c>
       <c r="B2898" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C2898" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C2898" t="inlineStr"/>
     </row>
     <row r="2899">
       <c r="A2899" t="n">
@@ -36684,7 +36344,7 @@
       </c>
       <c r="B2918" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C2918" t="inlineStr">
@@ -38118,11 +37778,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C3035" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C3035" t="inlineStr"/>
     </row>
     <row r="3036">
       <c r="A3036" t="n">
@@ -38130,7 +37786,7 @@
       </c>
       <c r="B3036" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3036" t="inlineStr">
@@ -38610,11 +38266,7 @@
       <c r="A3074" t="n">
         <v>4528310</v>
       </c>
-      <c r="B3074" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B3074" t="inlineStr"/>
       <c r="C3074" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -39047,14 +38699,10 @@
       </c>
       <c r="B3107" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C3107" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3107" t="inlineStr"/>
     </row>
     <row r="3108">
       <c r="A3108" t="n">
@@ -39191,7 +38839,7 @@
       </c>
       <c r="B3119" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3119" t="inlineStr">
@@ -39206,7 +38854,7 @@
       </c>
       <c r="B3120" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3120" t="inlineStr">
@@ -39357,14 +39005,10 @@
       </c>
       <c r="B3133" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C3133" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3133" t="inlineStr"/>
     </row>
     <row r="3134">
       <c r="A3134" t="n">
@@ -39605,14 +39249,10 @@
       </c>
       <c r="B3153" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C3153" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3153" t="inlineStr"/>
     </row>
     <row r="3154">
       <c r="A3154" t="n">
@@ -39945,7 +39585,7 @@
       </c>
       <c r="B3181" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3181" t="inlineStr">
@@ -40133,14 +39773,10 @@
       </c>
       <c r="B3197" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECAR EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C3197" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3197" t="inlineStr"/>
     </row>
     <row r="3198">
       <c r="A3198" t="n">
@@ -40148,14 +39784,10 @@
       </c>
       <c r="B3198" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C3198" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3198" t="inlineStr"/>
     </row>
     <row r="3199">
       <c r="A3199" t="n">
@@ -40787,7 +40419,7 @@
       </c>
       <c r="B3247" t="inlineStr">
         <is>
-          <t>LEYENDA DE CENTRIFUGADO</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C3247" t="inlineStr">
@@ -40802,7 +40434,7 @@
       </c>
       <c r="B3248" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3248" t="inlineStr">
@@ -40815,11 +40447,7 @@
       <c r="A3249" t="n">
         <v>4560171</v>
       </c>
-      <c r="B3249" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B3249" t="inlineStr"/>
       <c r="C3249" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -42311,11 +41939,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C3374" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C3374" t="inlineStr"/>
     </row>
     <row r="3375">
       <c r="A3375" t="n">
@@ -42768,7 +42392,7 @@
       </c>
       <c r="B3410" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3410" t="inlineStr">
@@ -43158,11 +42782,7 @@
       <c r="A3442" t="n">
         <v>4654594</v>
       </c>
-      <c r="B3442" t="inlineStr">
-        <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
+      <c r="B3442" t="inlineStr"/>
       <c r="C3442" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -43663,11 +43283,7 @@
       <c r="A3485" t="n">
         <v>4693490</v>
       </c>
-      <c r="B3485" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B3485" t="inlineStr"/>
       <c r="C3485" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -44505,14 +44121,10 @@
       </c>
       <c r="B3557" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C3557" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3557" t="inlineStr"/>
     </row>
     <row r="3558">
       <c r="A3558" t="n">
@@ -45157,7 +44769,7 @@
       </c>
       <c r="B3613" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3613" t="inlineStr">
@@ -46377,7 +45989,7 @@
       </c>
       <c r="B3717" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>INSTRUCCIONES</t>
         </is>
       </c>
       <c r="C3717" t="inlineStr">
@@ -46390,11 +46002,7 @@
       <c r="A3718" t="n">
         <v>4767627</v>
       </c>
-      <c r="B3718" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B3718" t="inlineStr"/>
       <c r="C3718" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -46695,7 +46303,7 @@
       </c>
       <c r="B3743" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C3743" t="inlineStr">
@@ -47083,14 +46691,10 @@
       </c>
       <c r="B3775" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C3775" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3775" t="inlineStr"/>
     </row>
     <row r="3776">
       <c r="A3776" t="n">
@@ -47611,11 +47215,7 @@
           <t>INSTRUCCIONES</t>
         </is>
       </c>
-      <c r="C3818" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C3818" t="inlineStr"/>
     </row>
     <row r="3819">
       <c r="A3819" t="n">
@@ -47887,14 +47487,10 @@
       </c>
       <c r="B3839" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C3839" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C3839" t="inlineStr"/>
     </row>
     <row r="3840">
       <c r="A3840" t="n">
@@ -48434,11 +48030,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C3883" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C3883" t="inlineStr"/>
     </row>
     <row r="3884">
       <c r="A3884" t="n">
@@ -48687,14 +48279,10 @@
       </c>
       <c r="B3903" t="inlineStr">
         <is>
-          <t>SIN</t>
-        </is>
-      </c>
-      <c r="C3903" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C3903" t="inlineStr"/>
     </row>
     <row r="3904">
       <c r="A3904" t="n">
@@ -48702,7 +48290,7 @@
       </c>
       <c r="B3904" t="inlineStr">
         <is>
-          <t>SIN</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C3904" t="inlineStr">
@@ -50095,7 +49683,7 @@
       </c>
       <c r="B4015" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4015" t="inlineStr">
@@ -50933,7 +50521,7 @@
       </c>
       <c r="B4085" t="inlineStr">
         <is>
-          <t>SE EVALUA CON NOM 004</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4085" t="inlineStr">
@@ -50963,14 +50551,10 @@
       </c>
       <c r="B4087" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C4087" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C4087" t="inlineStr"/>
     </row>
     <row r="4088">
       <c r="A4088" t="n">
@@ -51509,11 +51093,7 @@
       <c r="A4135" t="n">
         <v>4871310</v>
       </c>
-      <c r="B4135" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4135" t="inlineStr"/>
       <c r="C4135" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -51524,11 +51104,7 @@
       <c r="A4136" t="n">
         <v>4871311</v>
       </c>
-      <c r="B4136" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4136" t="inlineStr"/>
       <c r="C4136" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -52232,11 +51808,7 @@
       <c r="A4196" t="n">
         <v>4879990</v>
       </c>
-      <c r="B4196" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECAR EN LINEA A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4196" t="inlineStr"/>
       <c r="C4196" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -52397,7 +51969,7 @@
       </c>
       <c r="B4209" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4209" t="inlineStr">
@@ -52412,7 +51984,7 @@
       </c>
       <c r="B4210" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4210" t="inlineStr">
@@ -52515,14 +52087,10 @@
       </c>
       <c r="B4219" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C4219" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C4219" t="inlineStr"/>
     </row>
     <row r="4220">
       <c r="A4220" t="n">
@@ -53583,7 +53151,7 @@
       </c>
       <c r="B4303" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4303" t="inlineStr">
@@ -54037,11 +53605,7 @@
       <c r="A4343" t="n">
         <v>4923840</v>
       </c>
-      <c r="B4343" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B4343" t="inlineStr"/>
       <c r="C4343" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -54669,7 +54233,7 @@
       </c>
       <c r="B4393" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4393" t="inlineStr">
@@ -55864,11 +55428,7 @@
       <c r="A4496" t="n">
         <v>4967628</v>
       </c>
-      <c r="B4496" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4496" t="inlineStr"/>
       <c r="C4496" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -56989,7 +56549,7 @@
       </c>
       <c r="B4593" t="inlineStr">
         <is>
-          <t>SIN</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4593" t="inlineStr">
@@ -57100,14 +56660,10 @@
       </c>
       <c r="B4602" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C4602" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C4602" t="inlineStr"/>
     </row>
     <row r="4603">
       <c r="A4603" t="n">
@@ -57306,11 +56862,7 @@
       <c r="A4618" t="n">
         <v>4997645</v>
       </c>
-      <c r="B4618" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4618" t="inlineStr"/>
       <c r="C4618" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -58966,11 +58518,7 @@
       <c r="A4754" t="n">
         <v>5025029</v>
       </c>
-      <c r="B4754" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B4754" t="inlineStr"/>
       <c r="C4754" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -59101,7 +58649,7 @@
       </c>
       <c r="B4765" t="inlineStr">
         <is>
-          <t>NO DECLARA INSUMO DE CINTAS</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4765" t="inlineStr">
@@ -60331,11 +59879,7 @@
       <c r="A4869" t="n">
         <v>5054326</v>
       </c>
-      <c r="B4869" t="inlineStr">
-        <is>
-          <t>SIN</t>
-        </is>
-      </c>
+      <c r="B4869" t="inlineStr"/>
       <c r="C4869" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -60484,14 +60028,10 @@
       </c>
       <c r="B4882" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C4882" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C4882" t="inlineStr"/>
     </row>
     <row r="4883">
       <c r="A4883" t="n">
@@ -60945,7 +60485,7 @@
       </c>
       <c r="B4921" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4921" t="inlineStr">
@@ -61049,14 +60589,10 @@
       </c>
       <c r="B4929" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C4929" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C4929" t="inlineStr"/>
     </row>
     <row r="4930">
       <c r="A4930" t="n">
@@ -61525,7 +61061,7 @@
       </c>
       <c r="B4969" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECAR EN LINEA A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C4969" t="inlineStr">
@@ -63706,11 +63242,7 @@
       <c r="A5150" t="n">
         <v>5104620</v>
       </c>
-      <c r="B5150" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B5150" t="inlineStr"/>
       <c r="C5150" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -64029,11 +63561,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C5176" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C5176" t="inlineStr"/>
     </row>
     <row r="5177">
       <c r="A5177" t="n">
@@ -64110,11 +63638,7 @@
           <t>REVISADO</t>
         </is>
       </c>
-      <c r="C5183" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C5183" t="inlineStr"/>
     </row>
     <row r="5184">
       <c r="A5184" t="n">
@@ -64644,7 +64168,7 @@
       </c>
       <c r="B5230" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C5230" t="inlineStr">
@@ -65314,11 +64838,7 @@
       <c r="A5286" t="n">
         <v>5165502</v>
       </c>
-      <c r="B5286" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B5286" t="inlineStr"/>
       <c r="C5286" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -65715,7 +65235,7 @@
       </c>
       <c r="B5319" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C5319" t="inlineStr">
@@ -65776,11 +65296,7 @@
       <c r="A5324" t="n">
         <v>5177883</v>
       </c>
-      <c r="B5324" t="inlineStr">
-        <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
+      <c r="B5324" t="inlineStr"/>
       <c r="C5324" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -66713,14 +66229,10 @@
       </c>
       <c r="B5405" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
-        </is>
-      </c>
-      <c r="C5405" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C5405" t="inlineStr"/>
     </row>
     <row r="5406">
       <c r="A5406" t="n">
@@ -66728,14 +66240,10 @@
       </c>
       <c r="B5406" t="inlineStr">
         <is>
-          <t>No exprimir, no centrifugar y secado en línea a la sombra.</t>
-        </is>
-      </c>
-      <c r="C5406" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C5406" t="inlineStr"/>
     </row>
     <row r="5407">
       <c r="A5407" t="n">
@@ -72801,7 +72309,7 @@
       </c>
       <c r="B5933" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C5933" t="inlineStr">
@@ -75662,7 +75170,7 @@
       </c>
       <c r="B6184" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>CUMPLE</t>
         </is>
       </c>
       <c r="C6184" t="inlineStr"/>
@@ -77332,14 +76840,10 @@
       </c>
       <c r="B6334" t="inlineStr">
         <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
-      <c r="C6334" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C6334" t="inlineStr"/>
     </row>
     <row r="6335">
       <c r="A6335" t="n">
@@ -78669,7 +78173,7 @@
       </c>
       <c r="B6449" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C6449" t="inlineStr">
@@ -78830,11 +78334,7 @@
           <t>IMPORTADOR, EDAD</t>
         </is>
       </c>
-      <c r="C6463" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C6463" t="inlineStr"/>
     </row>
     <row r="6464">
       <c r="A6464" t="n">
@@ -79115,7 +78615,7 @@
       </c>
       <c r="B6487" t="inlineStr">
         <is>
-          <t>SIN</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C6487" t="inlineStr">
@@ -82169,7 +81669,7 @@
       </c>
       <c r="B6753" t="inlineStr">
         <is>
-          <t>NO EXPRIMIR NO CENTRIFUGAR SECADO EN LINEAL A LA SOMBRA</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C6753" t="inlineStr">
@@ -84358,7 +83858,7 @@
       </c>
       <c r="B6944" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C6944" t="inlineStr">
@@ -84552,11 +84052,7 @@
       <c r="A6960" t="n">
         <v>5514206</v>
       </c>
-      <c r="B6960" t="inlineStr">
-        <is>
-          <t>SIN</t>
-        </is>
-      </c>
+      <c r="B6960" t="inlineStr"/>
       <c r="C6960" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -84582,11 +84078,7 @@
       <c r="A6962" t="n">
         <v>5514208</v>
       </c>
-      <c r="B6962" t="inlineStr">
-        <is>
-          <t>SIN</t>
-        </is>
-      </c>
+      <c r="B6962" t="inlineStr"/>
       <c r="C6962" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -84612,11 +84104,7 @@
       <c r="A6964" t="n">
         <v>5514841</v>
       </c>
-      <c r="B6964" t="inlineStr">
-        <is>
-          <t>SIN</t>
-        </is>
-      </c>
+      <c r="B6964" t="inlineStr"/>
       <c r="C6964" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -84638,11 +84126,7 @@
       <c r="A6966" t="n">
         <v>5514843</v>
       </c>
-      <c r="B6966" t="inlineStr">
-        <is>
-          <t>SIN</t>
-        </is>
-      </c>
+      <c r="B6966" t="inlineStr"/>
       <c r="C6966" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -85292,7 +84776,7 @@
       </c>
       <c r="B7022" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7022" t="inlineStr">
@@ -86105,7 +85589,7 @@
       </c>
       <c r="B7093" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7093" t="inlineStr">
@@ -86396,7 +85880,7 @@
       </c>
       <c r="B7118" t="inlineStr">
         <is>
-          <t>UNIDADES DE MEDIDA</t>
+          <t>CUMPLE</t>
         </is>
       </c>
       <c r="C7118" t="inlineStr"/>
@@ -86453,11 +85937,7 @@
       <c r="A7123" t="n">
         <v>5466960</v>
       </c>
-      <c r="B7123" t="inlineStr">
-        <is>
-          <t>PAIS,IMPORTADOR</t>
-        </is>
-      </c>
+      <c r="B7123" t="inlineStr"/>
       <c r="C7123" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -86548,14 +86028,10 @@
       </c>
       <c r="B7130" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7130" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7130" t="inlineStr"/>
     </row>
     <row r="7131">
       <c r="A7131" t="n">
@@ -86578,14 +86054,10 @@
       </c>
       <c r="B7132" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7132" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7132" t="inlineStr"/>
     </row>
     <row r="7133">
       <c r="A7133" t="n">
@@ -86623,14 +86095,10 @@
       </c>
       <c r="B7135" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C7135" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7135" t="inlineStr"/>
     </row>
     <row r="7136">
       <c r="A7136" t="n">
@@ -87165,7 +86633,7 @@
       </c>
       <c r="B7181" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA PAIS DE ORIGEN</t>
+          <t>CUMPLE</t>
         </is>
       </c>
       <c r="C7181" t="inlineStr"/>
@@ -87224,7 +86692,7 @@
       </c>
       <c r="B7186" t="inlineStr">
         <is>
-          <t>EDAD  RECOMENDADA IMPORTADOR UNIDAD DE MEDIDA</t>
+          <t>IMPORTADOR FALTA PAIS DE ORIGEN EN ESPAÑOL</t>
         </is>
       </c>
       <c r="C7186" t="inlineStr">
@@ -87239,14 +86707,10 @@
       </c>
       <c r="B7187" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7187" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7187" t="inlineStr"/>
     </row>
     <row r="7188">
       <c r="A7188" t="n">
@@ -87569,14 +87033,10 @@
       </c>
       <c r="B7213" t="inlineStr">
         <is>
-          <t>SE VALUA CON NOM 020</t>
-        </is>
-      </c>
-      <c r="C7213" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7213" t="inlineStr"/>
     </row>
     <row r="7214">
       <c r="A7214" t="n">
@@ -87906,11 +87366,7 @@
           <t>INSTRUCCIONES</t>
         </is>
       </c>
-      <c r="C7239" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C7239" t="inlineStr"/>
     </row>
     <row r="7240">
       <c r="A7240" t="n">
@@ -87918,14 +87374,10 @@
       </c>
       <c r="B7240" t="inlineStr">
         <is>
-          <t>SE EVALUA CON LA N0M 020 Y CUMPLE</t>
-        </is>
-      </c>
-      <c r="C7240" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7240" t="inlineStr"/>
     </row>
     <row r="7241">
       <c r="A7241" t="n">
@@ -88085,7 +87537,7 @@
       </c>
       <c r="B7253" t="inlineStr">
         <is>
-          <t>SE EVALUA CON NOM 020</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7253" t="inlineStr">
@@ -88510,7 +87962,7 @@
       </c>
       <c r="B7288" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7288" t="inlineStr">
@@ -88649,11 +88101,7 @@
           <t>INSTRUCCIONES</t>
         </is>
       </c>
-      <c r="C7300" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C7300" t="inlineStr"/>
     </row>
     <row r="7301">
       <c r="A7301" t="n">
@@ -89560,14 +89008,10 @@
       </c>
       <c r="B7378" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C7378" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7378" t="inlineStr"/>
     </row>
     <row r="7379">
       <c r="A7379" t="n">
@@ -89584,11 +89028,7 @@
       <c r="A7380" t="n">
         <v>4899428</v>
       </c>
-      <c r="B7380" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
+      <c r="B7380" t="inlineStr"/>
       <c r="C7380" t="inlineStr">
         <is>
           <t>REVISADO</t>
@@ -89653,7 +89093,7 @@
       </c>
       <c r="B7385" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7385" t="inlineStr">
@@ -89668,7 +89108,7 @@
       </c>
       <c r="B7386" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7386" t="inlineStr">
@@ -90970,7 +90410,7 @@
       </c>
       <c r="B7500" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7500" t="inlineStr">
@@ -91069,11 +90509,7 @@
           <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
-      <c r="C7508" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+      <c r="C7508" t="inlineStr"/>
     </row>
     <row r="7509">
       <c r="A7509" t="n">
@@ -91162,7 +90598,7 @@
       </c>
       <c r="B7516" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7516" t="inlineStr">
@@ -91177,7 +90613,7 @@
       </c>
       <c r="B7517" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7517" t="inlineStr">
@@ -91214,7 +90650,7 @@
       </c>
       <c r="B7520" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7520" t="inlineStr">
@@ -91295,7 +90731,7 @@
       </c>
       <c r="B7527" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7527" t="inlineStr">
@@ -91461,7 +90897,7 @@
       </c>
       <c r="B7541" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7541" t="inlineStr">
@@ -91476,7 +90912,7 @@
       </c>
       <c r="B7542" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C7542" t="inlineStr">
@@ -91898,10 +91334,14 @@
       </c>
       <c r="B7576" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
-        </is>
-      </c>
-      <c r="C7576" t="inlineStr"/>
+          <t>INSTRUCCIONES</t>
+        </is>
+      </c>
+      <c r="C7576" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
     </row>
     <row r="7577">
       <c r="A7577" t="n">
@@ -92108,14 +91548,10 @@
       </c>
       <c r="B7594" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C7594" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7594" t="inlineStr"/>
     </row>
     <row r="7595">
       <c r="A7595" t="n">
@@ -92123,14 +91559,10 @@
       </c>
       <c r="B7595" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C7595" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7595" t="inlineStr"/>
     </row>
     <row r="7596">
       <c r="A7596" t="n">
@@ -92138,14 +91570,10 @@
       </c>
       <c r="B7596" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES</t>
-        </is>
-      </c>
-      <c r="C7596" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7596" t="inlineStr"/>
     </row>
     <row r="7597">
       <c r="A7597" t="n">
@@ -92191,7 +91619,7 @@
       </c>
       <c r="C7600" t="inlineStr">
         <is>
-          <t>REVISADO</t>
+          <t>IMPORTADOR</t>
         </is>
       </c>
     </row>
@@ -92206,7 +91634,7 @@
       </c>
       <c r="C7601" t="inlineStr">
         <is>
-          <t>REVISADO</t>
+          <t>IMPORTADOR</t>
         </is>
       </c>
     </row>
@@ -92221,7 +91649,7 @@
       </c>
       <c r="C7602" t="inlineStr">
         <is>
-          <t>REVISADO</t>
+          <t>INSUMOS</t>
         </is>
       </c>
     </row>
@@ -92447,7 +91875,7 @@
       </c>
       <c r="B7619" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7619" t="inlineStr">
@@ -92533,14 +91961,10 @@
       </c>
       <c r="B7625" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
-        </is>
-      </c>
-      <c r="C7625" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7625" t="inlineStr"/>
     </row>
     <row r="7626">
       <c r="A7626" t="n">
@@ -92600,7 +92024,7 @@
       </c>
       <c r="B7630" t="inlineStr">
         <is>
-          <t>ADVERTENCIAS</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7630" t="inlineStr">
@@ -92750,14 +92174,10 @@
       </c>
       <c r="B7640" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA</t>
-        </is>
-      </c>
-      <c r="C7640" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7640" t="inlineStr"/>
     </row>
     <row r="7641">
       <c r="A7641" t="n">
@@ -92840,7 +92260,7 @@
       </c>
       <c r="B7646" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7646" t="inlineStr">
@@ -92870,48 +92290,36 @@
       </c>
       <c r="B7648" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7648" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7648" t="inlineStr"/>
     </row>
     <row r="7649">
       <c r="A7649" t="n">
-        <v>5326515</v>
+        <v>4868697</v>
       </c>
       <c r="B7649" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7649" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7649" t="inlineStr"/>
     </row>
     <row r="7650">
       <c r="A7650" t="n">
-        <v>4924282</v>
+        <v>4994331</v>
       </c>
       <c r="B7650" t="inlineStr">
         <is>
-          <t>IMPORTADOR, PAIS</t>
-        </is>
-      </c>
-      <c r="C7650" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7650" t="inlineStr"/>
     </row>
     <row r="7651">
       <c r="A7651" t="n">
-        <v>2075400</v>
+        <v>5055652</v>
       </c>
       <c r="B7651" t="inlineStr">
         <is>
@@ -92922,7 +92330,7 @@
     </row>
     <row r="7652">
       <c r="A7652" t="n">
-        <v>5644563</v>
+        <v>5055653</v>
       </c>
       <c r="B7652" t="inlineStr">
         <is>
@@ -92933,7 +92341,7 @@
     </row>
     <row r="7653">
       <c r="A7653" t="n">
-        <v>5644564</v>
+        <v>5153886</v>
       </c>
       <c r="B7653" t="inlineStr">
         <is>
@@ -92944,22 +92352,18 @@
     </row>
     <row r="7654">
       <c r="A7654" t="n">
-        <v>2879877</v>
+        <v>4514405</v>
       </c>
       <c r="B7654" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7654" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7654" t="inlineStr"/>
     </row>
     <row r="7655">
       <c r="A7655" t="n">
-        <v>5167449</v>
+        <v>4514406</v>
       </c>
       <c r="B7655" t="inlineStr">
         <is>
@@ -92970,18 +92374,22 @@
     </row>
     <row r="7656">
       <c r="A7656" t="n">
-        <v>5167450</v>
+        <v>4098623</v>
       </c>
       <c r="B7656" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
-        </is>
-      </c>
-      <c r="C7656" t="inlineStr"/>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7656" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
     </row>
     <row r="7657">
       <c r="A7657" t="n">
-        <v>5644570</v>
+        <v>4560127</v>
       </c>
       <c r="B7657" t="inlineStr">
         <is>
@@ -92992,22 +92400,18 @@
     </row>
     <row r="7658">
       <c r="A7658" t="n">
-        <v>4131939</v>
+        <v>4954495</v>
       </c>
       <c r="B7658" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7658" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7658" t="inlineStr"/>
     </row>
     <row r="7659">
       <c r="A7659" t="n">
-        <v>5158324</v>
+        <v>4954496</v>
       </c>
       <c r="B7659" t="inlineStr">
         <is>
@@ -93018,7 +92422,7 @@
     </row>
     <row r="7660">
       <c r="A7660" t="n">
-        <v>5158327</v>
+        <v>5255859</v>
       </c>
       <c r="B7660" t="inlineStr">
         <is>
@@ -93029,7 +92433,7 @@
     </row>
     <row r="7661">
       <c r="A7661" t="n">
-        <v>5644560</v>
+        <v>4548894</v>
       </c>
       <c r="B7661" t="inlineStr">
         <is>
@@ -93040,7 +92444,7 @@
     </row>
     <row r="7662">
       <c r="A7662" t="n">
-        <v>4098622</v>
+        <v>4269016</v>
       </c>
       <c r="B7662" t="inlineStr">
         <is>
@@ -93055,7 +92459,7 @@
     </row>
     <row r="7663">
       <c r="A7663" t="n">
-        <v>4433705</v>
+        <v>4404592</v>
       </c>
       <c r="B7663" t="inlineStr">
         <is>
@@ -93066,7 +92470,7 @@
     </row>
     <row r="7664">
       <c r="A7664" t="n">
-        <v>5166910</v>
+        <v>4004495</v>
       </c>
       <c r="B7664" t="inlineStr">
         <is>
@@ -93077,11 +92481,11 @@
     </row>
     <row r="7665">
       <c r="A7665" t="n">
-        <v>5304434</v>
+        <v>5044430</v>
       </c>
       <c r="B7665" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>IMPOTADOR PAIS EDAD</t>
         </is>
       </c>
       <c r="C7665" t="inlineStr">
@@ -93092,82 +92496,62 @@
     </row>
     <row r="7666">
       <c r="A7666" t="n">
-        <v>5304435</v>
+        <v>5418879</v>
       </c>
       <c r="B7666" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7666" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7666" t="inlineStr"/>
     </row>
     <row r="7667">
       <c r="A7667" t="n">
-        <v>5304436</v>
+        <v>4781433</v>
       </c>
       <c r="B7667" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7667" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7667" t="inlineStr"/>
     </row>
     <row r="7668">
       <c r="A7668" t="n">
-        <v>5304438</v>
+        <v>5058912</v>
       </c>
       <c r="B7668" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7668" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7668" t="inlineStr"/>
     </row>
     <row r="7669">
       <c r="A7669" t="n">
-        <v>5304439</v>
+        <v>5144561</v>
       </c>
       <c r="B7669" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7669" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7669" t="inlineStr"/>
     </row>
     <row r="7670">
       <c r="A7670" t="n">
-        <v>5304440</v>
+        <v>4467254</v>
       </c>
       <c r="B7670" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7670" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7670" t="inlineStr"/>
     </row>
     <row r="7671">
       <c r="A7671" t="n">
-        <v>5664476</v>
+        <v>2080885</v>
       </c>
       <c r="B7671" t="inlineStr">
         <is>
@@ -93178,11 +92562,11 @@
     </row>
     <row r="7672">
       <c r="A7672" t="n">
-        <v>5010504</v>
+        <v>4667095</v>
       </c>
       <c r="B7672" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
+          <t>IMPOTADOR PAIS EDAD</t>
         </is>
       </c>
       <c r="C7672" t="inlineStr">
@@ -93193,7 +92577,7 @@
     </row>
     <row r="7673">
       <c r="A7673" t="n">
-        <v>5443795</v>
+        <v>4975198</v>
       </c>
       <c r="B7673" t="inlineStr">
         <is>
@@ -93204,122 +92588,114 @@
     </row>
     <row r="7674">
       <c r="A7674" t="n">
-        <v>5104597</v>
+        <v>1541614</v>
       </c>
       <c r="B7674" t="inlineStr">
         <is>
-          <t>INSTRUCCIONES DE CUIDADO</t>
-        </is>
-      </c>
-      <c r="C7674" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7674" t="inlineStr"/>
     </row>
     <row r="7675">
       <c r="A7675" t="n">
-        <v>4467254</v>
+        <v>5166856</v>
       </c>
       <c r="B7675" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7675" t="inlineStr"/>
     </row>
     <row r="7676">
       <c r="A7676" t="n">
-        <v>5094832</v>
+        <v>5155414</v>
       </c>
       <c r="B7676" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7676" t="inlineStr"/>
     </row>
     <row r="7677">
       <c r="A7677" t="n">
-        <v>2218122</v>
+        <v>5158613</v>
       </c>
       <c r="B7677" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7677" t="inlineStr"/>
     </row>
     <row r="7678">
       <c r="A7678" t="n">
-        <v>2611362</v>
+        <v>2955006</v>
       </c>
       <c r="B7678" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7678" t="inlineStr"/>
     </row>
     <row r="7679">
       <c r="A7679" t="n">
-        <v>4593087</v>
+        <v>5553722</v>
       </c>
       <c r="B7679" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
+          <t>REVISADO</t>
         </is>
       </c>
       <c r="C7679" t="inlineStr"/>
     </row>
     <row r="7680">
       <c r="A7680" t="n">
-        <v>5229944</v>
+        <v>4016200</v>
       </c>
       <c r="B7680" t="inlineStr">
         <is>
-          <t>CUMPLE</t>
-        </is>
-      </c>
-      <c r="C7680" t="inlineStr"/>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7680" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
     </row>
     <row r="7681">
       <c r="A7681" t="n">
-        <v>2379503</v>
+        <v>4838919</v>
       </c>
       <c r="B7681" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA PAIS DE ORIGEN</t>
-        </is>
-      </c>
-      <c r="C7681" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7681" t="inlineStr"/>
     </row>
     <row r="7682">
       <c r="A7682" t="n">
-        <v>4486688</v>
+        <v>5295153</v>
       </c>
       <c r="B7682" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7682" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>REVISADO</t>
+        </is>
+      </c>
+      <c r="C7682" t="inlineStr"/>
     </row>
     <row r="7683">
       <c r="A7683" t="n">
-        <v>2406881</v>
+        <v>4567165</v>
       </c>
       <c r="B7683" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C7683" t="inlineStr">
@@ -93330,11 +92706,11 @@
     </row>
     <row r="7684">
       <c r="A7684" t="n">
-        <v>2583663</v>
+        <v>5419268</v>
       </c>
       <c r="B7684" t="inlineStr">
         <is>
-          <t>EDAR RECOMENDADA UNIDAD DE MEDIDA</t>
+          <t>EDAD RECOMENDADA</t>
         </is>
       </c>
       <c r="C7684" t="inlineStr">
@@ -93345,26 +92721,22 @@
     </row>
     <row r="7685">
       <c r="A7685" t="n">
-        <v>4527518</v>
+        <v>4954494</v>
       </c>
       <c r="B7685" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
-        </is>
-      </c>
-      <c r="C7685" t="inlineStr">
-        <is>
-          <t>REVISADO</t>
-        </is>
-      </c>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7685" t="inlineStr"/>
     </row>
     <row r="7686">
       <c r="A7686" t="n">
-        <v>4667091</v>
+        <v>4964945</v>
       </c>
       <c r="B7686" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA IMPORTADOR UNIDAD DE MEDIDA</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C7686" t="inlineStr">
@@ -93375,11 +92747,11 @@
     </row>
     <row r="7687">
       <c r="A7687" t="n">
-        <v>4934021</v>
+        <v>2404873</v>
       </c>
       <c r="B7687" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
+          <t>EDAD RECOMENDADA</t>
         </is>
       </c>
       <c r="C7687" t="inlineStr">
@@ -93390,11 +92762,11 @@
     </row>
     <row r="7688">
       <c r="A7688" t="n">
-        <v>5264921</v>
+        <v>5217344</v>
       </c>
       <c r="B7688" t="inlineStr">
         <is>
-          <t>EDAD RECOMENDADA UNIDAD DE MEDIDA IMPORTADOR</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C7688" t="inlineStr">
@@ -93405,11 +92777,11 @@
     </row>
     <row r="7689">
       <c r="A7689" t="n">
-        <v>4375862</v>
+        <v>2880417</v>
       </c>
       <c r="B7689" t="inlineStr">
         <is>
-          <t>IMPORTADOR</t>
+          <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
       <c r="C7689" t="inlineStr">
@@ -93420,14 +92792,392 @@
     </row>
     <row r="7690">
       <c r="A7690" t="n">
-        <v>885266</v>
+        <v>4645933</v>
       </c>
       <c r="B7690" t="inlineStr">
         <is>
+          <t>CARACTERISTICAS ELECTRICAS</t>
+        </is>
+      </c>
+      <c r="C7690" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7691">
+      <c r="A7691" t="n">
+        <v>4351200</v>
+      </c>
+      <c r="B7691" t="inlineStr">
+        <is>
+          <t>EDAD RECOMENDADA IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7691" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7692">
+      <c r="A7692" t="n">
+        <v>2471317</v>
+      </c>
+      <c r="B7692" t="inlineStr">
+        <is>
           <t>INSTRUCCIONES DE CUIDADO</t>
         </is>
       </c>
-      <c r="C7690" t="inlineStr">
+      <c r="C7692" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7693">
+      <c r="A7693" t="n">
+        <v>2354661</v>
+      </c>
+      <c r="B7693" t="inlineStr"/>
+      <c r="C7693" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7694">
+      <c r="A7694" t="n">
+        <v>4169366</v>
+      </c>
+      <c r="B7694" t="inlineStr">
+        <is>
+          <t>EDAD RECOMENDADA</t>
+        </is>
+      </c>
+      <c r="C7694" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7695">
+      <c r="A7695" t="n">
+        <v>4228783</v>
+      </c>
+      <c r="B7695" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7695" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7696">
+      <c r="A7696" t="n">
+        <v>333642</v>
+      </c>
+      <c r="B7696" t="inlineStr">
+        <is>
+          <t>INSUMOS</t>
+        </is>
+      </c>
+      <c r="C7696" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7697">
+      <c r="A7697" t="n">
+        <v>4557828</v>
+      </c>
+      <c r="B7697" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7697" t="inlineStr"/>
+    </row>
+    <row r="7698">
+      <c r="A7698" t="n">
+        <v>4267562</v>
+      </c>
+      <c r="B7698" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7698" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7699">
+      <c r="A7699" t="n">
+        <v>4494450</v>
+      </c>
+      <c r="B7699" t="inlineStr">
+        <is>
+          <t>CUMPLE</t>
+        </is>
+      </c>
+      <c r="C7699" t="inlineStr"/>
+    </row>
+    <row r="7700">
+      <c r="A7700" t="n">
+        <v>5134046</v>
+      </c>
+      <c r="B7700" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7700" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7701">
+      <c r="A7701" t="n">
+        <v>4997375</v>
+      </c>
+      <c r="B7701" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7701" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7702">
+      <c r="A7702" t="n">
+        <v>4788497</v>
+      </c>
+      <c r="B7702" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7702" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7703">
+      <c r="A7703" t="n">
+        <v>5057380</v>
+      </c>
+      <c r="B7703" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7703" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7704">
+      <c r="A7704" t="n">
+        <v>5165504</v>
+      </c>
+      <c r="B7704" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7704" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7705">
+      <c r="A7705" t="n">
+        <v>5419576</v>
+      </c>
+      <c r="B7705" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7705" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7706">
+      <c r="A7706" t="n">
+        <v>4772553</v>
+      </c>
+      <c r="B7706" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7706" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7707">
+      <c r="A7707" t="n">
+        <v>5503694</v>
+      </c>
+      <c r="B7707" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7707" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7708">
+      <c r="A7708" t="n">
+        <v>4533407</v>
+      </c>
+      <c r="B7708" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7708" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7709">
+      <c r="A7709" t="n">
+        <v>4560113</v>
+      </c>
+      <c r="B7709" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7709" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7710">
+      <c r="A7710" t="n">
+        <v>4560114</v>
+      </c>
+      <c r="B7710" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7710" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7711">
+      <c r="A7711" t="n">
+        <v>2665774</v>
+      </c>
+      <c r="B7711" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7711" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7712">
+      <c r="A7712" t="n">
+        <v>2665775</v>
+      </c>
+      <c r="B7712" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7712" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7713">
+      <c r="A7713" t="n">
+        <v>2354657</v>
+      </c>
+      <c r="B7713" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7713" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7714">
+      <c r="A7714" t="n">
+        <v>2750076</v>
+      </c>
+      <c r="B7714" t="inlineStr">
+        <is>
+          <t>IMPORTADOR</t>
+        </is>
+      </c>
+      <c r="C7714" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7715">
+      <c r="A7715" t="n">
+        <v>2955008</v>
+      </c>
+      <c r="B7715" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7715" t="inlineStr">
+        <is>
+          <t>REVISADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7716">
+      <c r="A7716" t="n">
+        <v>4261780</v>
+      </c>
+      <c r="B7716" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES DE CUIDADO</t>
+        </is>
+      </c>
+      <c r="C7716" t="inlineStr">
         <is>
           <t>REVISADO</t>
         </is>

</xml_diff>